<commit_message>
Epi Info7: Extended to the logic driving the creation of a new project from data Dictionary.
</commit_message>
<xml_diff>
--- a/Epi Info 7/Epi.Windows.MakeView/Excel/Survey.xlsx
+++ b/Epi Info 7/Epi.Windows.MakeView/Excel/Survey.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mii0\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\CDC\Workspace\Epi Info Web Survey\Epi.Web\Content\Text\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="18105" windowHeight="7680"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="18108" windowHeight="7680"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="41">
   <si>
     <t>Question</t>
   </si>
@@ -106,12 +106,6 @@
     <t>pregnant</t>
   </si>
   <si>
-    <t>Then_Question</t>
-  </si>
-  <si>
-    <t>Else_Question</t>
-  </si>
-  <si>
     <t>When did symptoms start?</t>
   </si>
   <si>
@@ -119,6 +113,45 @@
   </si>
   <si>
     <t>Date</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>Patient</t>
+  </si>
+  <si>
+    <t>Age</t>
+  </si>
+  <si>
+    <t>Pregnant</t>
+  </si>
+  <si>
+    <t>symptoms</t>
+  </si>
+  <si>
+    <t>Please enter Age ….</t>
+  </si>
+  <si>
+    <t>Please enter Name….</t>
+  </si>
+  <si>
+    <t>Please enter Sex….</t>
+  </si>
+  <si>
+    <t>Please enter Pregnant...</t>
+  </si>
+  <si>
+    <t>Please enter symptoms…</t>
+  </si>
+  <si>
+    <t>Title</t>
+  </si>
+  <si>
+    <t>Then_Goto</t>
+  </si>
+  <si>
+    <t>Else_Goto</t>
   </si>
 </sst>
 </file>
@@ -445,134 +478,171 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H6"/>
+  <dimension ref="A1:J6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="I1" sqref="I1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="26.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="26.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="26.109375" customWidth="1"/>
+    <col min="4" max="4" width="14.88671875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.5546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="G1" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I1" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>14</v>
       </c>
       <c r="B2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C2" t="s">
+        <v>34</v>
+      </c>
+      <c r="D2" t="s">
         <v>16</v>
       </c>
-      <c r="C2" t="s">
+      <c r="E2" t="s">
         <v>4</v>
       </c>
-      <c r="D2" t="b">
+      <c r="F2" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>17</v>
       </c>
       <c r="B3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C3" t="s">
+        <v>33</v>
+      </c>
+      <c r="D3" t="s">
         <v>18</v>
       </c>
-      <c r="C3" t="s">
+      <c r="E3" t="s">
         <v>5</v>
       </c>
-      <c r="D3" t="b">
+      <c r="F3" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>22</v>
       </c>
       <c r="B4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" t="s">
+        <v>35</v>
+      </c>
+      <c r="D4" t="s">
         <v>19</v>
       </c>
-      <c r="C4" t="s">
+      <c r="E4" t="s">
         <v>9</v>
       </c>
-      <c r="D4" t="b">
+      <c r="F4" t="b">
         <v>0</v>
       </c>
-      <c r="E4" t="s">
+      <c r="G4" t="s">
         <v>20</v>
       </c>
-      <c r="F4" t="s">
+      <c r="H4" t="s">
         <v>12</v>
       </c>
-      <c r="G4" t="s">
+      <c r="I4" t="s">
         <v>24</v>
       </c>
-      <c r="H4" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J4" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>23</v>
       </c>
       <c r="B5" t="s">
+        <v>31</v>
+      </c>
+      <c r="C5" t="s">
+        <v>36</v>
+      </c>
+      <c r="D5" t="s">
         <v>24</v>
       </c>
-      <c r="C5" t="s">
+      <c r="E5" t="s">
         <v>6</v>
       </c>
-      <c r="D5" t="b">
+      <c r="F5" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
+        <v>25</v>
+      </c>
+      <c r="B6" t="s">
+        <v>32</v>
+      </c>
+      <c r="C6" t="s">
+        <v>37</v>
+      </c>
+      <c r="D6" t="s">
+        <v>26</v>
+      </c>
+      <c r="E6" t="s">
         <v>27</v>
       </c>
-      <c r="B6" t="s">
-        <v>28</v>
-      </c>
-      <c r="C6" t="s">
-        <v>29</v>
-      </c>
-      <c r="D6" t="b">
+      <c r="F6" t="b">
         <v>1</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F1048576">
       <formula1>"TRUE,FALSE"</formula1>
     </dataValidation>
   </dataValidations>
@@ -585,7 +655,7 @@
           <x14:formula1>
             <xm:f>DataTypes!$A:$A</xm:f>
           </x14:formula1>
-          <xm:sqref>C2:C1048576</xm:sqref>
+          <xm:sqref>E2:E1048576</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -601,24 +671,24 @@
       <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>13</v>
       </c>
@@ -636,41 +706,41 @@
       <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
[EI-979] Changed “Then_Goto” and “Else_Goto” to “Then_Question” and “Else_Question” in the Survey.xlsx data dictionary.
</commit_message>
<xml_diff>
--- a/Epi Info 7/Epi.Windows.MakeView/Excel/Survey.xlsx
+++ b/Epi Info 7/Epi.Windows.MakeView/Excel/Survey.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\CDC\Workspace\Epi Info Web Survey\Epi.Web\Content\Text\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\TFSCode\Epi Info 7\Epi.Windows.MakeView\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="18108" windowHeight="7680"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="18105" windowHeight="7680"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -148,10 +148,10 @@
     <t>Title</t>
   </si>
   <si>
-    <t>Then_Goto</t>
-  </si>
-  <si>
-    <t>Else_Goto</t>
+    <t>Then_Question</t>
+  </si>
+  <si>
+    <t>Else_Question</t>
   </si>
 </sst>
 </file>
@@ -481,22 +481,22 @@
   <dimension ref="A1:J6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I1" sqref="I1"/>
+      <selection activeCell="L10" sqref="L10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="26.109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="26.109375" customWidth="1"/>
-    <col min="4" max="4" width="14.88671875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="26.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="26.140625" customWidth="1"/>
+    <col min="4" max="4" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.5703125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="11" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="12" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="14.6640625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="13.88671875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -528,7 +528,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>14</v>
       </c>
@@ -548,7 +548,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>17</v>
       </c>
@@ -568,7 +568,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>22</v>
       </c>
@@ -600,7 +600,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>23</v>
       </c>
@@ -620,7 +620,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>25</v>
       </c>
@@ -671,24 +671,24 @@
       <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>13</v>
       </c>
@@ -706,39 +706,39 @@
       <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>27</v>
       </c>

</xml_diff>

<commit_message>
[EI-979] [Rollback] Changed “then_goto” and “else_goto” to “then_question” and “else_question” in the survey.xlsx data dictionary.
</commit_message>
<xml_diff>
--- a/Epi Info 7/Epi.Windows.MakeView/Excel/Survey.xlsx
+++ b/Epi Info 7/Epi.Windows.MakeView/Excel/Survey.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\TFSCode\Epi Info 7\Epi.Windows.MakeView\Excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\CDC\Workspace\Epi Info Web Survey\Epi.Web\Content\Text\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="18105" windowHeight="7680"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="18108" windowHeight="7680"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -148,10 +148,10 @@
     <t>Title</t>
   </si>
   <si>
-    <t>Then_Question</t>
-  </si>
-  <si>
-    <t>Else_Question</t>
+    <t>Then_Goto</t>
+  </si>
+  <si>
+    <t>Else_Goto</t>
   </si>
 </sst>
 </file>
@@ -481,22 +481,22 @@
   <dimension ref="A1:J6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L10" sqref="L10"/>
+      <selection activeCell="I1" sqref="I1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="26.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="26.140625" customWidth="1"/>
-    <col min="4" max="4" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="26.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="26.109375" customWidth="1"/>
+    <col min="4" max="4" width="14.88671875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.5546875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="11" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="12" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -528,7 +528,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>14</v>
       </c>
@@ -548,7 +548,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>17</v>
       </c>
@@ -568,7 +568,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>22</v>
       </c>
@@ -600,7 +600,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>23</v>
       </c>
@@ -620,7 +620,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>25</v>
       </c>
@@ -671,24 +671,24 @@
       <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>13</v>
       </c>
@@ -706,39 +706,39 @@
       <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>27</v>
       </c>

</xml_diff>

<commit_message>
updated the Excel template.
</commit_message>
<xml_diff>
--- a/Epi Info 7/Epi.Windows.MakeView/Excel/Survey.xlsx
+++ b/Epi Info 7/Epi.Windows.MakeView/Excel/Survey.xlsx
@@ -5,16 +5,18 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\CDC\Workspace\Epi Info Web Survey\Epi.Web\Content\Text\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mii0\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="18108" windowHeight="7680"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId2"/>
-    <sheet name="DataTypes" sheetId="2" r:id="rId3"/>
+    <sheet name="Sheet4" sheetId="5" r:id="rId2"/>
+    <sheet name="Sheet2" sheetId="4" r:id="rId3"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId4"/>
+    <sheet name="DataTypes" sheetId="2" r:id="rId5"/>
   </sheets>
   <definedNames>
     <definedName name="Datatypes">DataTypes!$A$1:$A$6</definedName>
@@ -29,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="63">
   <si>
     <t>Question</t>
   </si>
@@ -127,9 +129,6 @@
     <t>Pregnant</t>
   </si>
   <si>
-    <t>symptoms</t>
-  </si>
-  <si>
     <t>Please enter Age ….</t>
   </si>
   <si>
@@ -142,9 +141,6 @@
     <t>Please enter Pregnant...</t>
   </si>
   <si>
-    <t>Please enter symptoms…</t>
-  </si>
-  <si>
     <t>Title</t>
   </si>
   <si>
@@ -152,6 +148,78 @@
   </si>
   <si>
     <t>Else_Goto</t>
+  </si>
+  <si>
+    <t>What time did the symptoms start?</t>
+  </si>
+  <si>
+    <t>Symptoms Date</t>
+  </si>
+  <si>
+    <t>Please enter symptoms date…</t>
+  </si>
+  <si>
+    <t>Symptoms Time</t>
+  </si>
+  <si>
+    <t>Please enter symptoms time…</t>
+  </si>
+  <si>
+    <t>onse_time</t>
+  </si>
+  <si>
+    <t>Time</t>
+  </si>
+  <si>
+    <t>Foods Eaten</t>
+  </si>
+  <si>
+    <t>eaten_foods</t>
+  </si>
+  <si>
+    <t>Sheet2</t>
+  </si>
+  <si>
+    <t>Fresh celery</t>
+  </si>
+  <si>
+    <t>Grapes</t>
+  </si>
+  <si>
+    <t>Peaches</t>
+  </si>
+  <si>
+    <t>Apple juice</t>
+  </si>
+  <si>
+    <t>Orange juice</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>Sheet4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Don't know </t>
+  </si>
+  <si>
+    <t>Select eaten foods:</t>
+  </si>
+  <si>
+    <t>Please select eaten foods…</t>
+  </si>
+  <si>
+    <t>Was patient hospitalized?</t>
+  </si>
+  <si>
+    <t>Hospitalization</t>
+  </si>
+  <si>
+    <t>hospitalized</t>
   </si>
 </sst>
 </file>
@@ -478,30 +546,29 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J6"/>
+  <dimension ref="A1:J9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I1" sqref="I1"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="26.109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="26.109375" customWidth="1"/>
-    <col min="4" max="4" width="14.88671875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="31.7109375" customWidth="1"/>
+    <col min="2" max="2" width="26.140625" customWidth="1"/>
+    <col min="3" max="3" width="33.42578125" customWidth="1"/>
+    <col min="4" max="4" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.5703125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="11" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="12" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="14.6640625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="13.88671875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>28</v>
@@ -522,13 +589,13 @@
         <v>21</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>14</v>
       </c>
@@ -536,7 +603,7 @@
         <v>29</v>
       </c>
       <c r="C2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D2" t="s">
         <v>16</v>
@@ -548,7 +615,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>17</v>
       </c>
@@ -556,7 +623,7 @@
         <v>30</v>
       </c>
       <c r="C3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D3" t="s">
         <v>18</v>
@@ -568,7 +635,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>22</v>
       </c>
@@ -576,7 +643,7 @@
         <v>10</v>
       </c>
       <c r="C4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D4" t="s">
         <v>19</v>
@@ -600,7 +667,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>23</v>
       </c>
@@ -608,7 +675,7 @@
         <v>31</v>
       </c>
       <c r="C5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D5" t="s">
         <v>24</v>
@@ -620,15 +687,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>25</v>
       </c>
       <c r="B6" t="s">
-        <v>32</v>
+        <v>40</v>
       </c>
       <c r="C6" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="D6" t="s">
         <v>26</v>
@@ -638,6 +705,69 @@
       </c>
       <c r="F6" t="b">
         <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>39</v>
+      </c>
+      <c r="B7" t="s">
+        <v>42</v>
+      </c>
+      <c r="C7" t="s">
+        <v>43</v>
+      </c>
+      <c r="D7" t="s">
+        <v>44</v>
+      </c>
+      <c r="E7" t="s">
+        <v>45</v>
+      </c>
+      <c r="F7" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>58</v>
+      </c>
+      <c r="B8" t="s">
+        <v>46</v>
+      </c>
+      <c r="C8" t="s">
+        <v>59</v>
+      </c>
+      <c r="D8" t="s">
+        <v>47</v>
+      </c>
+      <c r="E8" t="s">
+        <v>7</v>
+      </c>
+      <c r="F8" t="b">
+        <v>0</v>
+      </c>
+      <c r="G8" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>60</v>
+      </c>
+      <c r="B9" t="s">
+        <v>61</v>
+      </c>
+      <c r="D9" t="s">
+        <v>62</v>
+      </c>
+      <c r="E9" t="s">
+        <v>8</v>
+      </c>
+      <c r="F9" t="b">
+        <v>0</v>
+      </c>
+      <c r="G9" t="s">
+        <v>56</v>
       </c>
     </row>
   </sheetData>
@@ -665,32 +795,27 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A4"/>
+  <dimension ref="A1:A3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>13</v>
+        <v>57</v>
       </c>
     </row>
   </sheetData>
@@ -700,47 +825,127 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A7"/>
+  <dimension ref="A1:A5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>53</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>27</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>45</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Changed the "goto" statement on the EXCEL template
</commit_message>
<xml_diff>
--- a/Epi Info 7/Epi.Windows.MakeView/Excel/Survey.xlsx
+++ b/Epi Info 7/Epi.Windows.MakeView/Excel/Survey.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mii0\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\CDC\Workspace_EI7\Epi Info 7\epiinfo\Epi Info 7\Epi.Windows.MakeView\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12432"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="63">
   <si>
     <t>Question</t>
   </si>
@@ -548,22 +548,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J6" sqref="J6"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="31.7109375" customWidth="1"/>
-    <col min="2" max="2" width="26.140625" customWidth="1"/>
-    <col min="3" max="3" width="33.42578125" customWidth="1"/>
-    <col min="4" max="4" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="31.6640625" customWidth="1"/>
+    <col min="2" max="2" width="26.109375" customWidth="1"/>
+    <col min="3" max="3" width="33.44140625" customWidth="1"/>
+    <col min="4" max="4" width="14.88671875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.5546875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="11" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="12" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -595,7 +597,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>14</v>
       </c>
@@ -615,7 +617,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>17</v>
       </c>
@@ -635,7 +637,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>22</v>
       </c>
@@ -660,14 +662,14 @@
       <c r="H4" t="s">
         <v>12</v>
       </c>
-      <c r="I4" t="s">
-        <v>24</v>
-      </c>
-      <c r="J4" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="I4">
+        <v>4</v>
+      </c>
+      <c r="J4">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>23</v>
       </c>
@@ -687,7 +689,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>25</v>
       </c>
@@ -707,7 +709,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>39</v>
       </c>
@@ -727,7 +729,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>58</v>
       </c>
@@ -750,7 +752,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>60</v>
       </c>
@@ -801,19 +803,19 @@
       <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>57</v>
       </c>
@@ -831,29 +833,29 @@
       <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>53</v>
       </c>
@@ -871,24 +873,24 @@
       <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>13</v>
       </c>
@@ -906,44 +908,44 @@
       <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>45</v>
       </c>

</xml_diff>

<commit_message>
Changed 'onse_time' to 'onset_time' in Survey.xlsx.
</commit_message>
<xml_diff>
--- a/Epi Info 7/Epi.Windows.MakeView/Excel/Survey.xlsx
+++ b/Epi Info 7/Epi.Windows.MakeView/Excel/Survey.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mii0\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\TFSCode\Epi Info 7\Epi.Windows.MakeView\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -165,9 +165,6 @@
     <t>Please enter symptoms time…</t>
   </si>
   <si>
-    <t>onse_time</t>
-  </si>
-  <si>
     <t>Time</t>
   </si>
   <si>
@@ -220,12 +217,15 @@
   </si>
   <si>
     <t>hospitalized</t>
+  </si>
+  <si>
+    <t>onset_time</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -548,7 +548,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -718,10 +720,10 @@
         <v>43</v>
       </c>
       <c r="D7" t="s">
+        <v>62</v>
+      </c>
+      <c r="E7" t="s">
         <v>44</v>
-      </c>
-      <c r="E7" t="s">
-        <v>45</v>
       </c>
       <c r="F7" t="b">
         <v>0</v>
@@ -729,16 +731,16 @@
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
+        <v>57</v>
+      </c>
+      <c r="B8" t="s">
+        <v>45</v>
+      </c>
+      <c r="C8" t="s">
         <v>58</v>
       </c>
-      <c r="B8" t="s">
+      <c r="D8" t="s">
         <v>46</v>
-      </c>
-      <c r="C8" t="s">
-        <v>59</v>
-      </c>
-      <c r="D8" t="s">
-        <v>47</v>
       </c>
       <c r="E8" t="s">
         <v>7</v>
@@ -747,18 +749,18 @@
         <v>0</v>
       </c>
       <c r="G8" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
+        <v>59</v>
+      </c>
+      <c r="B9" t="s">
         <v>60</v>
       </c>
-      <c r="B9" t="s">
+      <c r="D9" t="s">
         <v>61</v>
-      </c>
-      <c r="D9" t="s">
-        <v>62</v>
       </c>
       <c r="E9" t="s">
         <v>8</v>
@@ -767,7 +769,7 @@
         <v>0</v>
       </c>
       <c r="G9" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
   </sheetData>
@@ -805,17 +807,17 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
   </sheetData>
@@ -835,27 +837,27 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
   </sheetData>
@@ -945,7 +947,7 @@
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
   </sheetData>

</xml_diff>